<commit_message>
new data and parsers
</commit_message>
<xml_diff>
--- a/data/Приложение №2.xlsx
+++ b/data/Приложение №2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="параметры программ" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Автор:
 </t>
@@ -50,7 +50,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">не включено в план-график</t>
         </r>
@@ -65,7 +65,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Автор:
 </t>
@@ -76,7 +76,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">не проводится на внешний рынок</t>
         </r>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="235">
   <si>
     <t xml:space="preserve">№ п\п</t>
   </si>
@@ -137,7 +137,23 @@
     <t xml:space="preserve"> Программа повышения квалификации "Центровка и контроль загрузки воздушных судов. Базовый курс"</t>
   </si>
   <si>
-    <t xml:space="preserve">требуется интерактивная доска</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">414б</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">80 </t>
@@ -159,7 +175,7 @@
     <t xml:space="preserve">Программа повышения квалификации государственных гражданских служащих, осуществляющих деятельность  в системе  управления и контроля безопасности  полетов аэропорта по теме:«Система управления безопасностью полетов аэропортов»</t>
   </si>
   <si>
-    <t xml:space="preserve">желательно все дни в одной и той же аудитории, может проводиться совместно с программой №4</t>
+    <t xml:space="preserve">no,,</t>
   </si>
   <si>
     <t xml:space="preserve"> 40</t>
@@ -168,9 +184,6 @@
     <t xml:space="preserve">Программа повышения квалификации  руководящего состава и специалистов поставщиков услуг по теме: "Система управления безопасностью полётов поставщиков услуг"</t>
   </si>
   <si>
-    <t xml:space="preserve">желательно все дни в одной и той же аудитории</t>
-  </si>
-  <si>
     <t xml:space="preserve">40 </t>
   </si>
   <si>
@@ -180,7 +193,7 @@
     <t xml:space="preserve">Программа повышения квалификации «Базовые компетенции преподавателей Авиационных учебных центров»</t>
   </si>
   <si>
-    <t xml:space="preserve">необходима аудитория  без парт: 414б-1 или 416аб</t>
+    <t xml:space="preserve">,,414б-1;416аб</t>
   </si>
   <si>
     <t xml:space="preserve"> 24</t>
@@ -196,9 +209,6 @@
   </si>
   <si>
     <t xml:space="preserve">Программа повышения квалификации «Перевозка опасных грузов воздушным транспортом. 10 категория ИКАО/ИАТА.Базовый курс»</t>
-  </si>
-  <si>
-    <t xml:space="preserve">нет</t>
   </si>
   <si>
     <t xml:space="preserve">Программа повышения квалификации «Перевозка опасных грузов воздушным транспортом. 10 категория ИКАО/ИАТА"</t>
@@ -250,13 +260,7 @@
     <t xml:space="preserve">Программа повышения квалификации «Организация наземного обслуживания воздушных судов.Базовый курс»</t>
   </si>
   <si>
-    <t xml:space="preserve">желателен  414б</t>
-  </si>
-  <si>
     <t xml:space="preserve">Программа повышения квалификации «Организация наземного обслуживания воздушных судов»</t>
-  </si>
-  <si>
-    <t xml:space="preserve">желателен 414б</t>
   </si>
   <si>
     <t xml:space="preserve">Противообледенительная
@@ -266,7 +270,7 @@
     <t xml:space="preserve">Программа повышения квалификации "Обеспечение противообледенительной защиты воздушных судов (категория по SAE AS6286А DI-L30).Базовый курс"</t>
   </si>
   <si>
-    <t xml:space="preserve">на практические занятия необходима аудитория БАТО,213</t>
+    <t xml:space="preserve">,,БАТО_213</t>
   </si>
   <si>
     <t xml:space="preserve">Программа повышения квалификации "Обеспечение противообледенительной защиты воздушных судов (категория по SAE AS6286А DI-L30)"</t>
@@ -287,9 +291,6 @@
     <t xml:space="preserve">Программа начальной подготовки водителей спецтранспорта без права подъезда к воздушному в контролируемой зоне аэродрома «Пулково»</t>
   </si>
   <si>
-    <t xml:space="preserve">аудитория БАТО,213</t>
-  </si>
-  <si>
     <t xml:space="preserve">Программа дополнительной подготовки водителей спецтранспорта без права подъезда к воздушному в контролируемой зоне аэродрома «Пулково»</t>
   </si>
   <si>
@@ -317,7 +318,7 @@
     <t xml:space="preserve">Программа начальной подготовки «Предполётный досмотр пассажиров, членов экипажей гражданских судов, обслуживающего персонала, ручной клади, багажа, грузов, почты и бортовых запасов»</t>
   </si>
   <si>
-    <t xml:space="preserve">аудитория 105,106,107</t>
+    <t xml:space="preserve">,,105;106;107</t>
   </si>
   <si>
     <t xml:space="preserve">Программа специальной профессиональной подготовки «Предполётный досмотр пассажиров, членов экипажей гражданских судов, обслуживающего персонала, ручной клади, багажа, грузов, почты и бортовых запасов»</t>
@@ -350,7 +351,7 @@
     <t xml:space="preserve">Аварийно-спасательное обеспечение полетов</t>
   </si>
   <si>
-    <t xml:space="preserve">ГАСС</t>
+    <t xml:space="preserve">,,ГАСС</t>
   </si>
   <si>
     <t xml:space="preserve">Аудитрия</t>
@@ -398,10 +399,13 @@
     <t xml:space="preserve">стулья без парт, для тренинговых форматов</t>
   </si>
   <si>
+    <t xml:space="preserve">нет</t>
+  </si>
+  <si>
     <t xml:space="preserve">все дисциплины</t>
   </si>
   <si>
-    <t xml:space="preserve">416а,б</t>
+    <t xml:space="preserve">416аб</t>
   </si>
   <si>
     <t xml:space="preserve">практические</t>
@@ -415,14 +419,17 @@
 только для практических занятий по программам №30, 31 и 32</t>
   </si>
   <si>
-    <t xml:space="preserve">ИАС, 202</t>
+    <t xml:space="preserve">ГАСС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИАС_202</t>
   </si>
   <si>
     <t xml:space="preserve">Организация наземного обслуживания;
 Центровка и контроль загрузки</t>
   </si>
   <si>
-    <t xml:space="preserve">БАТО, 213</t>
+    <t xml:space="preserve">БАТО_213</t>
   </si>
   <si>
     <t xml:space="preserve">Водители; ПОЗ ВС</t>
@@ -458,7 +465,7 @@
     <t xml:space="preserve">1;2</t>
   </si>
   <si>
-    <t xml:space="preserve">все темы</t>
+    <t xml:space="preserve">,,1;2,2</t>
   </si>
   <si>
     <t xml:space="preserve">пятидневный</t>
@@ -470,6 +477,9 @@
     <t xml:space="preserve">Красненко А.Г.</t>
   </si>
   <si>
+    <t xml:space="preserve">,,1;2,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">32909</t>
   </si>
   <si>
@@ -482,18 +492,27 @@
     <t xml:space="preserve">3;4</t>
   </si>
   <si>
+    <t xml:space="preserve">,,3;4,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">40825</t>
   </si>
   <si>
     <t xml:space="preserve">Корнеев Р.Л.</t>
   </si>
   <si>
+    <t xml:space="preserve">,,3;4,2</t>
+  </si>
+  <si>
     <t xml:space="preserve">42927</t>
   </si>
   <si>
     <t xml:space="preserve">Чернов Д.А.</t>
   </si>
   <si>
+    <t xml:space="preserve">,,3;4,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">12426</t>
   </si>
   <si>
@@ -503,6 +522,9 @@
     <t xml:space="preserve">7;8;11;12</t>
   </si>
   <si>
+    <t xml:space="preserve">,,7;8;11;12,2</t>
+  </si>
+  <si>
     <t xml:space="preserve">сменный</t>
   </si>
   <si>
@@ -515,7 +537,7 @@
     <t xml:space="preserve">Шабалин К.Н.</t>
   </si>
   <si>
-    <t xml:space="preserve">при распределении на программы 7 и 8 - приоритет 1</t>
+    <t xml:space="preserve">,,7;8,1</t>
   </si>
   <si>
     <t xml:space="preserve">35684</t>
@@ -527,7 +549,7 @@
     <t xml:space="preserve">11;12</t>
   </si>
   <si>
-    <t xml:space="preserve">при распределении на программы 11 и 12- приоритет 1</t>
+    <t xml:space="preserve">,,11;12,1</t>
   </si>
   <si>
     <t xml:space="preserve">37590</t>
@@ -542,7 +564,7 @@
     <t xml:space="preserve">11;12;9;10;13;14</t>
   </si>
   <si>
-    <t xml:space="preserve">при распределении на программы 11;12 приоритет 2</t>
+    <t xml:space="preserve">,,11;12,2</t>
   </si>
   <si>
     <t xml:space="preserve">6841</t>
@@ -560,10 +582,10 @@
     <t xml:space="preserve">30;31;32;33;34;35;36;37;38;39</t>
   </si>
   <si>
-    <t xml:space="preserve">если заняты преподаватели Монахов Г.П., Умняшкин О.В., Щеглов А.В., Морозов Д.В</t>
-  </si>
-  <si>
-    <t xml:space="preserve">за исключением тем с 4 раздела в программе 34 и  тем с раздела 8 в программе 35</t>
+    <t xml:space="preserve">,,30;31;32;33;34;35;36;37;38;39,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!&gt;3:34;!&gt;7:35</t>
   </si>
   <si>
     <t xml:space="preserve">39275</t>
@@ -572,7 +594,7 @@
     <t xml:space="preserve">Монахов Г.П.</t>
   </si>
   <si>
-    <t xml:space="preserve">в рабочие смены</t>
+    <t xml:space="preserve">,,30;31;32;33;34;35;36;37;38;39,1</t>
   </si>
   <si>
     <t xml:space="preserve">3/4 смена</t>
@@ -593,7 +615,10 @@
     <t xml:space="preserve">34;35</t>
   </si>
   <si>
-    <t xml:space="preserve">только разделы с 4 по программе 34, разделы с 8 на программе 35</t>
+    <t xml:space="preserve">,,34;35,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;3:34;&gt;7:35</t>
   </si>
   <si>
     <t xml:space="preserve">27294</t>
@@ -602,6 +627,9 @@
     <t xml:space="preserve">Красиков А.В.</t>
   </si>
   <si>
+    <t xml:space="preserve">,,34;35,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">33292</t>
   </si>
   <si>
@@ -620,7 +648,7 @@
     <t xml:space="preserve">31;32</t>
   </si>
   <si>
-    <t xml:space="preserve">если нет других свободных преподавателей</t>
+    <t xml:space="preserve">,,31;32,5</t>
   </si>
   <si>
     <t xml:space="preserve">37734</t>
@@ -663,6 +691,9 @@
     <t xml:space="preserve">Биднюк В.Д.</t>
   </si>
   <si>
+    <t xml:space="preserve">,,,</t>
+  </si>
+  <si>
     <t xml:space="preserve">25059</t>
   </si>
   <si>
@@ -699,7 +730,7 @@
     <t xml:space="preserve">17;18;19;20</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - на теоретические занятия, 2 - на практические</t>
+    <t xml:space="preserve">1,2,,</t>
   </si>
   <si>
     <t xml:space="preserve">32708</t>
@@ -720,10 +751,7 @@
     <t xml:space="preserve">Патешкин В.Ю.</t>
   </si>
   <si>
-    <t xml:space="preserve">1- на практические занятия, 2 на теоретические</t>
-  </si>
-  <si>
-    <t xml:space="preserve">в первую очередь - практические занятия</t>
+    <t xml:space="preserve">2,1,,</t>
   </si>
   <si>
     <t xml:space="preserve">36258</t>
@@ -738,7 +766,7 @@
     <t xml:space="preserve">Кушниренко П.В.</t>
   </si>
   <si>
-    <t xml:space="preserve">все теоретические занятия</t>
+    <t xml:space="preserve">1,5,,</t>
   </si>
   <si>
     <t xml:space="preserve">37636</t>
@@ -750,12 +778,18 @@
     <t xml:space="preserve">15;16</t>
   </si>
   <si>
+    <t xml:space="preserve">,,15;16,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">40080</t>
   </si>
   <si>
     <t xml:space="preserve">Суббота П.В.</t>
   </si>
   <si>
+    <t xml:space="preserve">,,15;16,2</t>
+  </si>
+  <si>
     <t xml:space="preserve">43312</t>
   </si>
   <si>
@@ -765,6 +799,9 @@
     <t xml:space="preserve">5;6</t>
   </si>
   <si>
+    <t xml:space="preserve">,,5;6,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">6811</t>
   </si>
   <si>
@@ -775,6 +812,9 @@
   </si>
   <si>
     <t xml:space="preserve">13;14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,,13;14,1</t>
   </si>
 </sst>
 </file>
@@ -783,10 +823,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]#,##0_);[RED]\(#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="[$-409]#,##0\ ;[RED]\(#,##0\)"/>
     <numFmt numFmtId="166" formatCode="[$-409]D\-MMM"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -813,19 +853,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
       <family val="0"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -833,6 +873,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -846,14 +891,14 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -861,21 +906,21 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -883,7 +928,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -977,7 +1022,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,7 +1055,7 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1026,27 +1071,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1054,11 +1099,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1066,7 +1115,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1085,6 +1134,13 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1092,6 +1148,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1099,6 +1162,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1106,6 +1176,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1113,6 +1190,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1120,6 +1204,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1127,6 +1218,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1134,6 +1232,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1215,19 +1320,20 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="C1" activeCellId="1" sqref="12:12 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="149.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="5" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="15" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1319,7 +1425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
@@ -1407,7 +1513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
@@ -1416,13 +1522,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>18</v>
@@ -1450,24 +1556,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>24</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>18</v>
@@ -1495,22 +1601,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
@@ -1543,19 +1649,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>24</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>18</v>
@@ -1583,22 +1689,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>18</v>
@@ -1626,22 +1732,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>18</v>
@@ -1669,22 +1775,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>18</v>
@@ -1712,22 +1818,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>18</v>
@@ -1755,22 +1861,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>18</v>
@@ -1803,25 +1909,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>16</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>2</v>
@@ -1843,28 +1949,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>32</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I15" s="5" t="n">
         <v>4</v>
@@ -1891,13 +1997,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>72</v>
@@ -1931,16 +2037,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>32</v>
@@ -1979,13 +2085,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>16</v>
@@ -2019,16 +2125,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>16</v>
@@ -2062,16 +2168,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>16</v>
@@ -2105,16 +2211,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>16</v>
@@ -2154,7 +2260,7 @@
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="5" t="n">
@@ -2188,13 +2294,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>33</v>
@@ -2224,16 +2330,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>27</v>
@@ -2263,16 +2369,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>74</v>
@@ -2302,16 +2408,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>67</v>
@@ -2341,16 +2447,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>74</v>
@@ -2380,16 +2486,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>67</v>
@@ -2419,16 +2525,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>29.5</v>
@@ -2458,16 +2564,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>25.5</v>
@@ -2497,18 +2603,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E31" s="10" t="n">
         <v>144</v>
@@ -2541,16 +2647,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E32" s="10" t="n">
         <v>82</v>
@@ -2583,16 +2689,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E33" s="10" t="n">
         <v>42</v>
@@ -2625,16 +2731,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E34" s="10" t="n">
         <v>144</v>
@@ -2667,16 +2773,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E35" s="10" t="n">
         <v>82</v>
@@ -2709,16 +2815,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E36" s="10" t="n">
         <v>42</v>
@@ -2751,16 +2857,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E37" s="10" t="n">
         <v>144</v>
@@ -2793,16 +2899,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E38" s="10" t="n">
         <v>82</v>
@@ -2835,16 +2941,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E39" s="10" t="n">
         <v>42</v>
@@ -2877,16 +2983,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E40" s="10" t="n">
         <v>16</v>
@@ -2920,18 +3026,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E41" s="10" t="n">
         <v>136</v>
@@ -3036,11 +3142,11 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="12:12 A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -3048,29 +3154,30 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="7" style="0" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="n">
         <v>105</v>
       </c>
@@ -3078,19 +3185,19 @@
         <v>18</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="n">
         <v>106</v>
       </c>
@@ -3098,19 +3205,19 @@
         <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="n">
         <v>107</v>
       </c>
@@ -3118,79 +3225,79 @@
         <v>24</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>24</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>98</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B6" s="13" t="n">
         <v>32</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" s="13" t="n">
         <v>18</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>101</v>
-      </c>
       <c r="E7" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
         <v>422</v>
       </c>
@@ -3198,19 +3305,19 @@
         <v>18</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <v>3091</v>
       </c>
@@ -3218,76 +3325,76 @@
         <v>20</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B10" s="13" t="n">
         <v>20</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B11" s="13" t="n">
         <v>20</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="13" t="n">
         <v>18</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3308,153 +3415,147 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="12:12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="10" style="0" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="17" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>124</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="B5" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="C5" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>121</v>
-      </c>
+      <c r="F5" s="19"/>
       <c r="G5" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
         <v>131</v>
       </c>
@@ -3462,776 +3563,732 @@
         <v>132</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="19"/>
       <c r="G6" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="19"/>
       <c r="G7" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="E8" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="H13" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E15" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>184</v>
+        <v>187</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>188</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>189</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D22" s="18" t="n">
         <v>40</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F22" s="19"/>
       <c r="G22" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D23" s="18" t="n">
         <v>40</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D24" s="18" t="n">
         <v>40</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F24" s="19"/>
       <c r="G24" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D25" s="18" t="n">
         <v>40</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F25" s="19"/>
       <c r="G25" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F26" s="19"/>
       <c r="G26" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F27" s="19"/>
       <c r="G27" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="D28" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>200</v>
-      </c>
       <c r="E28" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F28" s="19"/>
       <c r="G28" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>209</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="F29" s="19"/>
       <c r="G29" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>209</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="F30" s="19"/>
       <c r="G30" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="F31" s="21" t="s">
-        <v>214</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="F31" s="22"/>
       <c r="G31" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E32" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="F32" s="19"/>
       <c r="G32" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E33" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" s="19"/>
       <c r="G33" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="E34" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="F34" s="19"/>
       <c r="G34" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="E35" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="19"/>
       <c r="G35" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>